<commit_message>
more updates to get sdusd sim to run
</commit_message>
<xml_diff>
--- a/R_code/model_xwalk_SDUSD.xlsx
+++ b/R_code/model_xwalk_SDUSD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nmath_000\Documents\Research\Heterogeneous-Teacher-Value-Added\R_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBA105E-2A7B-4A23-975A-8A1F9AAB8AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DBEB86-1842-41C6-B38C-CC73A9B5CB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11010" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="74715" yWindow="1770" windowWidth="21600" windowHeight="11010" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t xml:space="preserve">nsims </t>
   </si>
@@ -589,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R2">
         <v>0.9</v>
@@ -779,6 +779,326 @@
         <v>0.4</v>
       </c>
       <c r="Z2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0.3</v>
+      </c>
+      <c r="O3">
+        <v>0.6</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>5</v>
+      </c>
+      <c r="R3">
+        <v>0.9</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
+        <v>0.4</v>
+      </c>
+      <c r="V3">
+        <v>0.8</v>
+      </c>
+      <c r="W3">
+        <v>0.2</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>0.4</v>
+      </c>
+      <c r="Z3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0.3</v>
+      </c>
+      <c r="O4">
+        <v>0.6</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>0.9</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>0.4</v>
+      </c>
+      <c r="V4">
+        <v>0.8</v>
+      </c>
+      <c r="W4">
+        <v>0.2</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>0.4</v>
+      </c>
+      <c r="Z4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>500</v>
+      </c>
+      <c r="C5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0.3</v>
+      </c>
+      <c r="O5">
+        <v>0.6</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>0.9</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>0.4</v>
+      </c>
+      <c r="V5">
+        <v>0.8</v>
+      </c>
+      <c r="W5">
+        <v>0.2</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0.4</v>
+      </c>
+      <c r="Z5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.2</v>
+      </c>
+      <c r="G6">
+        <v>0.4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0.3</v>
+      </c>
+      <c r="O6">
+        <v>0.1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>0.9</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <v>0.4</v>
+      </c>
+      <c r="V6">
+        <v>0.8</v>
+      </c>
+      <c r="W6">
+        <v>0.2</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>0.4</v>
+      </c>
+      <c r="Z6">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>